<commit_message>
solve maximum number of events
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="221">
   <si>
     <t>Name</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-number-of-events-that-can-be-attended/</t>
+  </si>
+  <si>
+    <t>24/06/2024</t>
   </si>
   <si>
     <t>Product of Array Except Self</t>
@@ -1580,37 +1583,41 @@
       <c r="C27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="6"/>
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="F27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="6"/>
@@ -1618,13 +1625,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="6"/>
@@ -1632,13 +1639,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="6"/>
@@ -1646,13 +1653,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="6"/>
@@ -1660,13 +1667,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="6"/>
@@ -1674,13 +1681,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="6"/>
@@ -1688,13 +1695,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="6"/>
@@ -1702,13 +1709,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
@@ -1716,13 +1723,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="6"/>
@@ -1730,13 +1737,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
@@ -1748,13 +1755,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="6"/>
@@ -1762,13 +1769,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>31</v>
@@ -1778,31 +1785,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
       <c r="A42" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="6"/>
@@ -1810,13 +1817,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
       <c r="A43" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="6"/>
@@ -1824,13 +1831,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
       <c r="A44" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="6"/>
@@ -1838,13 +1845,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
       <c r="A45" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="6"/>
@@ -1852,13 +1859,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="6"/>
@@ -1866,13 +1873,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
       <c r="A47" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="6"/>
@@ -1880,13 +1887,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
       <c r="A48" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="6"/>
@@ -1894,13 +1901,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
       <c r="A49" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="6"/>
@@ -1908,13 +1915,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
       <c r="A50" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="6"/>
@@ -1922,13 +1929,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
       <c r="A51" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="6"/>
@@ -1936,13 +1943,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25">
       <c r="A52" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="6"/>
@@ -1950,13 +1957,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
       <c r="A53" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="6"/>
@@ -1964,13 +1971,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
       <c r="A54" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="6"/>
@@ -1978,31 +1985,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
       <c r="A55" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F55" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
       <c r="A56" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="6"/>
@@ -2010,13 +2017,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
       <c r="A57" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="6"/>
@@ -2024,13 +2031,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
       <c r="A58" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="6"/>
@@ -2038,13 +2045,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
       <c r="A59" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="6"/>
@@ -2052,13 +2059,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="6"/>
@@ -2066,13 +2073,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="6"/>
@@ -2080,13 +2087,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="6"/>
@@ -2094,13 +2101,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="6"/>
@@ -2108,13 +2115,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
       <c r="A64" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="6"/>
@@ -2122,13 +2129,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="20.25">
       <c r="A65" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="6"/>
@@ -2136,13 +2143,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="20.25">
       <c r="A66" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="6"/>
@@ -2150,13 +2157,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="20.25">
       <c r="A67" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="6"/>
@@ -2164,13 +2171,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="20.25">
       <c r="A68" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="6"/>
@@ -2178,13 +2185,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="20.25">
       <c r="A69" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="6"/>
@@ -2192,13 +2199,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="20.25">
       <c r="A70" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="6"/>
@@ -2206,13 +2213,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="20.25">
       <c r="A71" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="6"/>
@@ -2220,13 +2227,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="20.25">
       <c r="A72" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="6"/>
@@ -2234,13 +2241,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="20.25">
       <c r="A73" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="6"/>
@@ -2248,13 +2255,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="20.25">
       <c r="A74" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="6"/>
@@ -2262,13 +2269,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="20.25">
       <c r="A75" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="6"/>
@@ -2276,13 +2283,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="20.25">
       <c r="A76" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="6"/>
@@ -2290,13 +2297,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="20.25">
       <c r="A77" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="6"/>
@@ -2304,13 +2311,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="20.25">
       <c r="A78" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="6"/>
@@ -2318,13 +2325,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="20.25">
       <c r="A79" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="6"/>
@@ -2332,13 +2339,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="20.25">
       <c r="A80" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="6"/>
@@ -2346,13 +2353,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="20.25">
       <c r="A81" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="6"/>
@@ -2360,13 +2367,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="20.25">
       <c r="A82" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="6"/>
@@ -2374,13 +2381,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="20.25">
       <c r="A83" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
solve copy list with random pointer
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="221">
   <si>
     <t>Name</t>
   </si>
@@ -1619,8 +1619,12 @@
       <c r="C29" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="6"/>
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="F29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
solve reorganize string using max heap
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reorganize-string/</t>
+  </si>
+  <si>
+    <t>26/06/2024</t>
   </si>
   <si>
     <t>Consecutive Numbers Sum</t>
@@ -1976,19 +1979,23 @@
       <c r="C53" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="6"/>
+      <c r="D53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="F53" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>151</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="6"/>
@@ -1996,31 +2003,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F55" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="6"/>
@@ -2028,13 +2035,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="6"/>
@@ -2042,13 +2049,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
       <c r="A58" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="6"/>
@@ -2056,13 +2063,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
       <c r="A59" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="6"/>
@@ -2070,13 +2077,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="6"/>
@@ -2084,13 +2091,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="6"/>
@@ -2098,13 +2105,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="6"/>
@@ -2112,13 +2119,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="6"/>
@@ -2126,13 +2133,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
       <c r="A64" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="6"/>
@@ -2140,13 +2147,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="20.25">
       <c r="A65" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="6"/>
@@ -2154,13 +2161,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="20.25">
       <c r="A66" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="6"/>
@@ -2168,13 +2175,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="20.25">
       <c r="A67" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="6"/>
@@ -2182,13 +2189,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="20.25">
       <c r="A68" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="6"/>
@@ -2196,13 +2203,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="20.25">
       <c r="A69" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="6"/>
@@ -2210,13 +2217,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="20.25">
       <c r="A70" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="6"/>
@@ -2224,13 +2231,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="20.25">
       <c r="A71" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="6"/>
@@ -2238,13 +2245,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="20.25">
       <c r="A72" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="6"/>
@@ -2252,13 +2259,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="20.25">
       <c r="A73" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="6"/>
@@ -2266,13 +2273,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="20.25">
       <c r="A74" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="6"/>
@@ -2280,13 +2287,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="20.25">
       <c r="A75" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="6"/>
@@ -2294,13 +2301,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="20.25">
       <c r="A76" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="6"/>
@@ -2308,13 +2315,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="20.25">
       <c r="A77" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="6"/>
@@ -2322,13 +2329,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="20.25">
       <c r="A78" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="6"/>
@@ -2336,13 +2343,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="20.25">
       <c r="A79" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="6"/>
@@ -2350,13 +2357,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="20.25">
       <c r="A80" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="6"/>
@@ -2364,13 +2371,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="20.25">
       <c r="A81" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="6"/>
@@ -2378,13 +2385,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="20.25">
       <c r="A82" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="6"/>
@@ -2392,13 +2399,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="20.25">
       <c r="A83" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
solve Climbing Stars using Dynamic Programming
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -475,6 +475,9 @@
     <t>https://leetcode.com/problems/climbing-stairs/</t>
   </si>
   <si>
+    <t>26/06/2024</t>
+  </si>
+  <si>
     <t>Majority Element</t>
   </si>
   <si>
@@ -485,9 +488,6 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reorganize-string/</t>
-  </si>
-  <si>
-    <t>26/06/2024</t>
   </si>
   <si>
     <t>Consecutive Numbers Sum</t>
@@ -1951,19 +1951,23 @@
       <c r="C51" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="6"/>
+      <c r="D51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="F51" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>151</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="6"/>
@@ -1971,19 +1975,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>151</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F53" s="3"/>
     </row>

</xml_diff>

<commit_message>
solve kth smallest element in a sorted matrix using heap
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -2075,8 +2075,12 @@
       <c r="C59" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="6"/>
+      <c r="D59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="F59" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">

</xml_diff>

<commit_message>
solve capacity to ship package
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -2401,8 +2401,12 @@
       <c r="C82" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D82" s="4"/>
-      <c r="E82" s="6"/>
+      <c r="D82" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="F82" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="20.25">

</xml_diff>

<commit_message>
solve path sum 2
</commit_message>
<xml_diff>
--- a/Amazon_Coding_Problem_List.xlsx
+++ b/Amazon_Coding_Problem_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -2387,8 +2387,12 @@
       <c r="C81" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D81" s="4"/>
-      <c r="E81" s="6"/>
+      <c r="D81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="F81" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="20.25">

</xml_diff>